<commit_message>
Design IMU, Voltage Sensor, and Driver circuits
</commit_message>
<xml_diff>
--- a/pcb/datasheets/LED_resistors.xlsx
+++ b/pcb/datasheets/LED_resistors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhi\Downloads\pcb\STLink-Debug-Adaptor\electrical_design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abhi\Downloads\PCBs\Quadruped\pcb\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F84C7-10D2-455F-A0F4-BE5A463C30D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E666126-CCEF-4E49-96F1-67AC6946E947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="3405" windowWidth="21600" windowHeight="11295" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
+    <workbookView xWindow="2205" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{0DB087E7-7223-437B-8069-21B1D5F0AC0C}"/>
   </bookViews>
   <sheets>
     <sheet name="LED Resistor Calc" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>SMD</t>
   </si>
@@ -87,6 +87,24 @@
   </si>
   <si>
     <t>WHITE</t>
+  </si>
+  <si>
+    <t>JLCPCB</t>
+  </si>
+  <si>
+    <t>Yellow</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>C2297</t>
+  </si>
+  <si>
+    <t>C2286</t>
+  </si>
+  <si>
+    <t>C2296</t>
   </si>
 </sst>
 </file>
@@ -169,7 +187,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -237,9 +265,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>312254</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>90281</xdr:rowOff>
+      <xdr:colOff>350354</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>52181</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="5509113" cy="5172797"/>
     <xdr:pic>
@@ -263,7 +291,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="921854" y="1423781"/>
+          <a:off x="959954" y="2338181"/>
           <a:ext cx="5509113" cy="5172797"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -275,16 +303,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>676276</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>119232</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>52557</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>76853</xdr:rowOff>
+      <xdr:rowOff>29228</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -307,7 +335,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9525001" y="1733550"/>
+          <a:off x="10677526" y="1685925"/>
           <a:ext cx="605006" cy="2343803"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -617,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCEE65C-92B9-4F95-AF2E-8F9D1369F15D}">
-  <dimension ref="B3:L7"/>
+  <dimension ref="A3:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +664,7 @@
     <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>14</v>
       </c>
@@ -671,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
@@ -709,7 +737,7 @@
         <v>1.5058823529411767E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5" s="7"/>
       <c r="C5" s="4">
         <v>5</v>
@@ -745,7 +773,7 @@
         <v>1.5058823529411767E-2</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="4">
         <v>5</v>
@@ -781,7 +809,7 @@
         <v>1.5058823529411767E-2</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="7"/>
       <c r="C7" s="4">
         <v>3.3</v>
@@ -815,6 +843,123 @@
       <c r="L7" s="1">
         <f>(C7-F7)*K7*10^-3</f>
         <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="4">
+        <v>2.8</v>
+      </c>
+      <c r="G9" s="4">
+        <v>30</v>
+      </c>
+      <c r="H9" s="4">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3">
+        <f>(C9-F9)/(H9*10^-3)</f>
+        <v>440</v>
+      </c>
+      <c r="J9" s="4">
+        <v>470</v>
+      </c>
+      <c r="K9" s="2">
+        <f t="shared" ref="K9:K11" si="6">(C9-F9)/J9*10^3</f>
+        <v>4.6808510638297873</v>
+      </c>
+      <c r="L9" s="1">
+        <f t="shared" ref="L9:L11" si="7">(C9-F9)*K9*10^-3</f>
+        <v>1.0297872340425533E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="4">
+        <v>2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>100</v>
+      </c>
+      <c r="H10" s="4">
+        <v>20</v>
+      </c>
+      <c r="I10" s="3">
+        <f>(C10-F10)/(H10*10^-3)</f>
+        <v>64.999999999999986</v>
+      </c>
+      <c r="J10" s="4">
+        <v>75</v>
+      </c>
+      <c r="K10" s="2">
+        <f t="shared" si="6"/>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="L10" s="1">
+        <f t="shared" si="7"/>
+        <v>2.2533333333333329E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="4">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>100</v>
+      </c>
+      <c r="H11" s="4">
+        <v>20</v>
+      </c>
+      <c r="I11" s="3">
+        <f>(C11-F11)/(H11*10^-3)</f>
+        <v>64.999999999999986</v>
+      </c>
+      <c r="J11" s="4">
+        <v>75</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" si="6"/>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="7"/>
+        <v>2.2533333333333329E-2</v>
       </c>
     </row>
   </sheetData>
@@ -822,6 +967,11 @@
     <mergeCell ref="B4:B7"/>
   </mergeCells>
   <conditionalFormatting sqref="L4:L7">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+      <formula>0.25</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L9:L11">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.25</formula>
     </cfRule>

</xml_diff>